<commit_message>
Completed till Battery discharge
</commit_message>
<xml_diff>
--- a/TestingData/ConfigureData.xlsx
+++ b/TestingData/ConfigureData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Voc</t>
   </si>
@@ -36,6 +36,18 @@
   </si>
   <si>
     <t>Temp</t>
+  </si>
+  <si>
+    <t>21 V</t>
+  </si>
+  <si>
+    <t>3 A</t>
+  </si>
+  <si>
+    <t>322</t>
+  </si>
+  <si>
+    <t>100 %</t>
   </si>
 </sst>
 </file>
@@ -73,7 +85,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,7 +369,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -377,17 +389,17 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>18</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>50</v>
-      </c>
-      <c r="D2">
-        <v>322</v>
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>